<commit_message>
run on more subjects
</commit_message>
<xml_diff>
--- a/HR_Data/LWP2_0005_lab_timing.xlsx
+++ b/HR_Data/LWP2_0005_lab_timing.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18431"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\CDRIVE\CTPC\LIVEWELL WEARTECH WEARABILITY ALL\WEARTECH compiled participant timings with participant info\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sophie\Documents\MATLAB\HeartRate\HR_Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -15,7 +15,7 @@
     <sheet name="In Lab" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="171027"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -312,7 +312,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -696,10 +696,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O32"/>
+  <dimension ref="A1:L32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="M15" sqref="M15"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -711,12 +711,12 @@
     <col min="5" max="5" width="7.85546875" customWidth="1"/>
     <col min="6" max="6" width="16.7109375" customWidth="1"/>
     <col min="7" max="7" width="20.7109375" customWidth="1"/>
-    <col min="12" max="12" width="37" customWidth="1"/>
-    <col min="13" max="13" width="16.7109375" customWidth="1"/>
-    <col min="14" max="14" width="14.140625" customWidth="1"/>
+    <col min="9" max="9" width="37" customWidth="1"/>
+    <col min="10" max="10" width="16.7109375" customWidth="1"/>
+    <col min="11" max="11" width="14.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="C1" t="s">
         <v>13</v>
       </c>
@@ -726,11 +726,11 @@
       <c r="F1" t="s">
         <v>38</v>
       </c>
-      <c r="L1" s="10" t="s">
+      <c r="I1" s="10" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -744,7 +744,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>35</v>
       </c>
@@ -760,14 +760,14 @@
       <c r="G3" s="5">
         <v>0.58611111111111114</v>
       </c>
-      <c r="L3" t="s">
+      <c r="I3" t="s">
         <v>72</v>
       </c>
-      <c r="M3">
+      <c r="J3">
         <v>30</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>34</v>
       </c>
@@ -783,14 +783,14 @@
       <c r="G4" s="5">
         <v>0.58611111111111114</v>
       </c>
-      <c r="L4" t="s">
+      <c r="I4" t="s">
         <v>73</v>
       </c>
-      <c r="M4" t="s">
+      <c r="J4" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>14</v>
       </c>
@@ -806,14 +806,14 @@
       <c r="G5" s="6">
         <v>0.58680555555555558</v>
       </c>
-      <c r="L5" t="s">
+      <c r="I5" t="s">
         <v>75</v>
       </c>
-      <c r="M5" t="s">
+      <c r="J5" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>15</v>
       </c>
@@ -832,14 +832,14 @@
       <c r="G6" s="5">
         <v>0.58680555555555558</v>
       </c>
-      <c r="L6" t="s">
+      <c r="I6" t="s">
         <v>76</v>
       </c>
-      <c r="M6">
+      <c r="J6">
         <v>145</v>
       </c>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>16</v>
       </c>
@@ -858,17 +858,17 @@
       <c r="G7" s="5">
         <v>0.58750000000000002</v>
       </c>
-      <c r="L7" t="s">
+      <c r="I7" t="s">
         <v>77</v>
       </c>
-      <c r="N7" s="10" t="s">
+      <c r="K7" s="10" t="s">
         <v>78</v>
       </c>
-      <c r="O7" s="10" t="s">
+      <c r="L7" s="10" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>17</v>
       </c>
@@ -887,17 +887,17 @@
       <c r="G8" s="5">
         <v>0.58750000000000002</v>
       </c>
-      <c r="M8" s="10" t="s">
+      <c r="J8" s="10" t="s">
         <v>80</v>
       </c>
-      <c r="N8" t="s">
+      <c r="K8" t="s">
         <v>81</v>
       </c>
-      <c r="O8" t="s">
+      <c r="L8" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>18</v>
       </c>
@@ -919,17 +919,17 @@
       <c r="G9" s="5">
         <v>0.58750000000000002</v>
       </c>
-      <c r="M9" s="10" t="s">
+      <c r="J9" s="10" t="s">
         <v>82</v>
       </c>
-      <c r="N9" t="s">
+      <c r="K9" t="s">
         <v>90</v>
       </c>
-      <c r="O9" t="s">
+      <c r="L9" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>19</v>
       </c>
@@ -948,17 +948,17 @@
       <c r="G10" s="5">
         <v>0.58819444444444446</v>
       </c>
-      <c r="L10" t="s">
+      <c r="I10" t="s">
         <v>84</v>
       </c>
-      <c r="M10" t="s">
+      <c r="J10" t="s">
         <v>88</v>
       </c>
-      <c r="N10" t="s">
+      <c r="K10" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>20</v>
       </c>
@@ -977,14 +977,14 @@
       <c r="G11" s="5">
         <v>0.58819444444444446</v>
       </c>
-      <c r="L11" t="s">
+      <c r="I11" t="s">
         <v>85</v>
       </c>
-      <c r="M11" t="s">
+      <c r="J11" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>21</v>
       </c>
@@ -1007,7 +1007,7 @@
         <v>0.58819444444444446</v>
       </c>
     </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>22</v>
       </c>
@@ -1026,11 +1026,11 @@
       <c r="G13" s="6">
         <v>0.58888888888888891</v>
       </c>
-      <c r="L13" t="s">
+      <c r="I13" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>1</v>
       </c>
@@ -1049,14 +1049,14 @@
       <c r="G14" s="5">
         <v>0.58888888888888891</v>
       </c>
-      <c r="L14" t="s">
+      <c r="I14" t="s">
         <v>79</v>
       </c>
-      <c r="M14" t="s">
+      <c r="J14" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>2</v>
       </c>
@@ -1078,14 +1078,14 @@
       <c r="G15" s="5">
         <v>0.58958333333333335</v>
       </c>
-      <c r="L15" t="s">
+      <c r="I15" t="s">
         <v>78</v>
       </c>
-      <c r="M15" t="s">
+      <c r="J15" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>3</v>
       </c>

</xml_diff>